<commit_message>
Actualizacion excell T2 + modelo 2R2D
</commit_message>
<xml_diff>
--- a/Trabajo_2/IV_curves.xlsx
+++ b/Trabajo_2/IV_curves.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_6F86A283DF1F031CD3F39037392DA384C0D83113" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AE44437F-526E-4F49-9ED3-0241D37E4BDE}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTC France" sheetId="1" r:id="rId1"/>
@@ -15,14 +16,27 @@
     <sheet name="KC200GT2" sheetId="6" r:id="rId6"/>
     <sheet name="SPVSX5" sheetId="7" r:id="rId7"/>
     <sheet name="PSC" sheetId="8" r:id="rId8"/>
-    <sheet name="Hoja1" sheetId="9" r:id="rId9"/>
+    <sheet name="CTJ30" sheetId="10" r:id="rId9"/>
+    <sheet name="ATJ" sheetId="11" r:id="rId10"/>
+    <sheet name="Hoja1" sheetId="9" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="13">
   <si>
     <t>V</t>
   </si>
@@ -66,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,6 +156,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -189,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,9 +239,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,6 +291,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -432,7 +483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:B43"/>
   <sheetViews>
@@ -692,13 +743,952 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCAAC26-F4C5-4CF4-A2FD-FC163D329481}">
+  <dimension ref="A1:B101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>0.45400000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0.43099999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <f>B2/B1</f>
+        <v>0.94933920704845809</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <f>B3/B4</f>
+        <v>0.88461538461538447</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1.7857100000000001E-2</v>
+      </c>
+      <c r="B21">
+        <v>0.43208200000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5.3571399999999998E-2</v>
+      </c>
+      <c r="B22">
+        <v>0.43139899999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8.9285699999999996E-2</v>
+      </c>
+      <c r="B23">
+        <v>0.43139899999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.141234</v>
+      </c>
+      <c r="B24">
+        <v>0.43071700000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.17694799999999999</v>
+      </c>
+      <c r="B25">
+        <v>0.43139899999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.224026</v>
+      </c>
+      <c r="B26">
+        <v>0.43139899999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.33766200000000002</v>
+      </c>
+      <c r="B27">
+        <v>0.43071700000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.43181799999999998</v>
+      </c>
+      <c r="B28">
+        <v>0.43071700000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.49513000000000001</v>
+      </c>
+      <c r="B29">
+        <v>0.43139899999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.56655800000000001</v>
+      </c>
+      <c r="B30">
+        <v>0.43139899999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.65746800000000005</v>
+      </c>
+      <c r="B31">
+        <v>0.43071700000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.73701300000000003</v>
+      </c>
+      <c r="B32">
+        <v>0.43071700000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.81168799999999997</v>
+      </c>
+      <c r="B33">
+        <v>0.43071700000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.87337699999999996</v>
+      </c>
+      <c r="B34">
+        <v>0.43003400000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.94805200000000001</v>
+      </c>
+      <c r="B35">
+        <v>0.43071700000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1.0064900000000001</v>
+      </c>
+      <c r="B36">
+        <v>0.43003400000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1.0844199999999999</v>
+      </c>
+      <c r="B37">
+        <v>0.43071700000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1.1493500000000001</v>
+      </c>
+      <c r="B38">
+        <v>0.43071700000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1.18994</v>
+      </c>
+      <c r="B39">
+        <v>0.43139899999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1.22403</v>
+      </c>
+      <c r="B40">
+        <v>0.43208200000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1.2451300000000001</v>
+      </c>
+      <c r="B41">
+        <v>0.43276500000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1.28247</v>
+      </c>
+      <c r="B42">
+        <v>0.43139899999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1.32955</v>
+      </c>
+      <c r="B43">
+        <v>0.43071700000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1.35877</v>
+      </c>
+      <c r="B44">
+        <v>0.43003400000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1.3847400000000001</v>
+      </c>
+      <c r="B45">
+        <v>0.42935200000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1.45455</v>
+      </c>
+      <c r="B46">
+        <v>0.42866900000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1.48864</v>
+      </c>
+      <c r="B47">
+        <v>0.42866900000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1.5405800000000001</v>
+      </c>
+      <c r="B48">
+        <v>0.42935200000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1.59578</v>
+      </c>
+      <c r="B49">
+        <v>0.42935200000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1.6785699999999999</v>
+      </c>
+      <c r="B50">
+        <v>0.42935200000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1.7094199999999999</v>
+      </c>
+      <c r="B51">
+        <v>0.42730400000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1.76786</v>
+      </c>
+      <c r="B52">
+        <v>0.42662099999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1.8051900000000001</v>
+      </c>
+      <c r="B53">
+        <v>0.42662099999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1.86364</v>
+      </c>
+      <c r="B54">
+        <v>0.42525600000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1.9237</v>
+      </c>
+      <c r="B55">
+        <v>0.42593900000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1.96591</v>
+      </c>
+      <c r="B56">
+        <v>0.42593900000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2.02922</v>
+      </c>
+      <c r="B57">
+        <v>0.42593900000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2.0811700000000002</v>
+      </c>
+      <c r="B58">
+        <v>0.42525600000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2.1444800000000002</v>
+      </c>
+      <c r="B59">
+        <v>0.42662099999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2.1801900000000001</v>
+      </c>
+      <c r="B60">
+        <v>0.42593900000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2.2126600000000001</v>
+      </c>
+      <c r="B61">
+        <v>0.42662099999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2.2386400000000002</v>
+      </c>
+      <c r="B62">
+        <v>0.42389100000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2.2564899999999999</v>
+      </c>
+      <c r="B63">
+        <v>0.42184300000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2.2743500000000001</v>
+      </c>
+      <c r="B64">
+        <v>0.41706500000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2.2970799999999998</v>
+      </c>
+      <c r="B65">
+        <v>0.41433399999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2.31494</v>
+      </c>
+      <c r="B66">
+        <v>0.41023900000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2.3344200000000002</v>
+      </c>
+      <c r="B67">
+        <v>0.40409600000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2.3506499999999999</v>
+      </c>
+      <c r="B68">
+        <v>0.39727000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2.3668800000000001</v>
+      </c>
+      <c r="B69">
+        <v>0.39180900000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2.3798699999999999</v>
+      </c>
+      <c r="B70">
+        <v>0.38361800000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2.3961000000000001</v>
+      </c>
+      <c r="B71">
+        <v>0.37610900000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2.4107099999999999</v>
+      </c>
+      <c r="B72">
+        <v>0.36382300000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2.4237000000000002</v>
+      </c>
+      <c r="B73">
+        <v>0.35358400000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2.43344</v>
+      </c>
+      <c r="B74">
+        <v>0.34198000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2.4480499999999998</v>
+      </c>
+      <c r="B75">
+        <v>0.32901000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2.4577900000000001</v>
+      </c>
+      <c r="B76">
+        <v>0.31194499999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2.46591</v>
+      </c>
+      <c r="B77">
+        <v>0.30238900000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2.4788999999999999</v>
+      </c>
+      <c r="B78">
+        <v>0.28532400000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2.4918800000000001</v>
+      </c>
+      <c r="B79">
+        <v>0.27235500000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2.4951300000000001</v>
+      </c>
+      <c r="B80">
+        <v>0.25870300000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2.5</v>
+      </c>
+      <c r="B81">
+        <v>0.24846399999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2.5048699999999999</v>
+      </c>
+      <c r="B82">
+        <v>0.240956</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2.5113599999999998</v>
+      </c>
+      <c r="B83">
+        <v>0.23208200000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2.5162300000000002</v>
+      </c>
+      <c r="B84">
+        <v>0.22047800000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2.5211000000000001</v>
+      </c>
+      <c r="B85">
+        <v>0.20614299999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2.52922</v>
+      </c>
+      <c r="B86">
+        <v>0.19317400000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2.5373399999999999</v>
+      </c>
+      <c r="B87">
+        <v>0.17747399999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2.5405799999999998</v>
+      </c>
+      <c r="B88">
+        <v>0.16586999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>2.5454500000000002</v>
+      </c>
+      <c r="B89">
+        <v>0.14880499999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2.5503200000000001</v>
+      </c>
+      <c r="B90">
+        <v>0.13447100000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>2.56006</v>
+      </c>
+      <c r="B91">
+        <v>0.115358</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>2.5681799999999999</v>
+      </c>
+      <c r="B92">
+        <v>9.76109E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2.5762999999999998</v>
+      </c>
+      <c r="B93">
+        <v>7.6450500000000005E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>2.5795499999999998</v>
+      </c>
+      <c r="B94">
+        <v>5.8020500000000003E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2.5811700000000002</v>
+      </c>
+      <c r="B95">
+        <v>4.5733799999999998E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>2.5827900000000001</v>
+      </c>
+      <c r="B96">
+        <v>3.8907799999999999E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>2.5892900000000001</v>
+      </c>
+      <c r="B97">
+        <v>2.9351499999999999E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2.59091</v>
+      </c>
+      <c r="B98">
+        <v>1.9795199999999999E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2.59253</v>
+      </c>
+      <c r="B99">
+        <v>1.02389E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2.59416</v>
+      </c>
+      <c r="B100">
+        <v>2.0477799999999999E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>2.59416</v>
+      </c>
+      <c r="B101">
+        <v>-1.3651900000000001E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="B4:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.76049999999999995</v>
+      </c>
+      <c r="D4">
+        <v>0.52390000000000003</v>
+      </c>
+      <c r="E4">
+        <v>0.46279999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.5202</v>
+      </c>
+      <c r="G4">
+        <v>1.032</v>
+      </c>
+      <c r="H4">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="I4">
+        <v>0.50344</v>
+      </c>
+      <c r="J4">
+        <v>7.5514099999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0.68940000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.496</v>
+      </c>
+      <c r="E5">
+        <v>0.43890000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.50439999999999996</v>
+      </c>
+      <c r="G5">
+        <v>0.92549999999999999</v>
+      </c>
+      <c r="H5">
+        <v>7.61</v>
+      </c>
+      <c r="I5">
+        <v>0.48476000000000002</v>
+      </c>
+      <c r="J5">
+        <v>4.5378698640000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0.45069999999999999</v>
+      </c>
+      <c r="D6">
+        <v>2.27</v>
+      </c>
+      <c r="E6">
+        <v>2.41</v>
+      </c>
+      <c r="F6">
+        <v>2.411</v>
+      </c>
+      <c r="G6">
+        <v>12.493</v>
+      </c>
+      <c r="H6">
+        <v>26.3</v>
+      </c>
+      <c r="I6">
+        <v>12.099</v>
+      </c>
+      <c r="J6">
+        <v>0.56176000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0.57269999999999999</v>
+      </c>
+      <c r="D7">
+        <v>2.5649999999999999</v>
+      </c>
+      <c r="E7">
+        <v>2.726</v>
+      </c>
+      <c r="F7">
+        <v>2.7</v>
+      </c>
+      <c r="G7">
+        <v>16.777999999999999</v>
+      </c>
+      <c r="H7">
+        <v>32.9</v>
+      </c>
+      <c r="I7">
+        <v>13.574999999999999</v>
+      </c>
+      <c r="J7">
+        <v>0.75364900000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>0.906508875739645</v>
+      </c>
+      <c r="D8">
+        <v>0.94674556213017746</v>
+      </c>
+      <c r="E8">
+        <v>0.94835782195332763</v>
+      </c>
+      <c r="F8">
+        <v>0.96962706651287955</v>
+      </c>
+      <c r="G8">
+        <v>0.89680232558139528</v>
+      </c>
+      <c r="H8">
+        <v>0.92691839220462846</v>
+      </c>
+      <c r="I8">
+        <v>0.96289528047036399</v>
+      </c>
+      <c r="J8">
+        <v>0.60093013940442919</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>0.78697398288807408</v>
+      </c>
+      <c r="D9">
+        <v>0.8849902534113061</v>
+      </c>
+      <c r="E9">
+        <v>0.8840792369772561</v>
+      </c>
+      <c r="F9">
+        <v>0.89296296296296296</v>
+      </c>
+      <c r="G9">
+        <v>0.7446060317081894</v>
+      </c>
+      <c r="H9">
+        <v>0.79939209726443772</v>
+      </c>
+      <c r="I9">
+        <v>0.89127071823204429</v>
+      </c>
+      <c r="J9">
+        <v>0.74538677819515453</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>10.036772039939533</v>
+      </c>
+      <c r="D10">
+        <v>27.604770356564067</v>
+      </c>
+      <c r="E10">
+        <v>27.257431630195462</v>
+      </c>
+      <c r="F10">
+        <v>30.446017665662499</v>
+      </c>
+      <c r="G10">
+        <v>6.9374497552861518</v>
+      </c>
+      <c r="H10">
+        <v>11.081333500705474</v>
+      </c>
+      <c r="I10">
+        <v>29.826096878700085</v>
+      </c>
+      <c r="J10">
+        <v>9.3346715468244454</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:B82"/>
   <sheetViews>
     <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +2256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:B86"/>
   <sheetViews>
@@ -1873,11 +2863,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:B1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -9816,7 +10806,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:B44"/>
   <sheetViews>
@@ -10087,7 +11077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:B112"/>
   <sheetViews>
@@ -10902,7 +11892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:B1202"/>
   <sheetViews>
@@ -20437,7 +21427,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:B40"/>
   <sheetViews>
@@ -20676,216 +21666,743 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0C4865-135B-4D97-A370-21D25A448A27}">
+  <dimension ref="A1:B104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D16" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>0.76049999999999995</v>
-      </c>
-      <c r="D4">
-        <v>0.52390000000000003</v>
-      </c>
-      <c r="E4">
-        <v>0.46279999999999999</v>
-      </c>
-      <c r="F4">
-        <v>0.5202</v>
-      </c>
-      <c r="G4">
-        <v>1.032</v>
-      </c>
-      <c r="H4">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="I4">
-        <v>0.50344</v>
-      </c>
-      <c r="J4">
-        <v>7.5514099999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B1">
+        <v>0.47299999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>0.68940000000000001</v>
-      </c>
-      <c r="D5">
-        <v>0.496</v>
-      </c>
-      <c r="E5">
-        <v>0.43890000000000001</v>
-      </c>
-      <c r="F5">
-        <v>0.50439999999999996</v>
-      </c>
-      <c r="G5">
-        <v>0.92549999999999999</v>
-      </c>
-      <c r="H5">
-        <v>7.61</v>
-      </c>
-      <c r="I5">
-        <v>0.48476000000000002</v>
-      </c>
-      <c r="J5">
-        <v>4.5378698640000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B2">
+        <v>0.45400000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>0.45069999999999999</v>
-      </c>
-      <c r="D6">
-        <v>2.27</v>
-      </c>
-      <c r="E6">
-        <v>2.41</v>
-      </c>
-      <c r="F6">
-        <v>2.411</v>
-      </c>
-      <c r="G6">
-        <v>12.493</v>
-      </c>
-      <c r="H6">
-        <v>26.3</v>
-      </c>
-      <c r="I6">
-        <v>12.099</v>
-      </c>
-      <c r="J6">
-        <v>0.56176000000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B3">
+        <v>2.31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>0.57269999999999999</v>
-      </c>
-      <c r="D7">
-        <v>2.5649999999999999</v>
-      </c>
-      <c r="E7">
-        <v>2.726</v>
-      </c>
-      <c r="F7">
-        <v>2.7</v>
-      </c>
-      <c r="G7">
-        <v>16.777999999999999</v>
-      </c>
-      <c r="H7">
-        <v>32.9</v>
-      </c>
-      <c r="I7">
-        <v>13.574999999999999</v>
-      </c>
-      <c r="J7">
-        <v>0.75364900000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>0.906508875739645</v>
-      </c>
-      <c r="D8">
-        <v>0.94674556213017746</v>
-      </c>
-      <c r="E8">
-        <v>0.94835782195332763</v>
-      </c>
-      <c r="F8">
-        <v>0.96962706651287955</v>
-      </c>
-      <c r="G8">
-        <v>0.89680232558139528</v>
-      </c>
-      <c r="H8">
-        <v>0.92691839220462846</v>
-      </c>
-      <c r="I8">
-        <v>0.96289528047036399</v>
-      </c>
-      <c r="J8">
-        <v>0.60093013940442919</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>0.78697398288807408</v>
-      </c>
-      <c r="D9">
-        <v>0.8849902534113061</v>
-      </c>
-      <c r="E9">
-        <v>0.8840792369772561</v>
-      </c>
-      <c r="F9">
-        <v>0.89296296296296296</v>
-      </c>
-      <c r="G9">
-        <v>0.7446060317081894</v>
-      </c>
-      <c r="H9">
-        <v>0.79939209726443772</v>
-      </c>
-      <c r="I9">
-        <v>0.89127071823204429</v>
-      </c>
-      <c r="J9">
-        <v>0.74538677819515453</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>10.036772039939533</v>
-      </c>
-      <c r="D10">
-        <v>27.604770356564067</v>
-      </c>
-      <c r="E10">
-        <v>27.257431630195462</v>
-      </c>
-      <c r="F10">
-        <v>30.446017665662499</v>
-      </c>
-      <c r="G10">
-        <v>6.9374497552861518</v>
-      </c>
-      <c r="H10">
-        <v>11.081333500705474</v>
-      </c>
-      <c r="I10">
-        <v>29.826096878700085</v>
-      </c>
-      <c r="J10">
-        <v>9.3346715468244454</v>
+      <c r="B4">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <f>B2/B1</f>
+        <v>0.95983086680761109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <f>B3/B4</f>
+        <v>0.88505747126436785</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-2.0876599999999999E-3</v>
+      </c>
+      <c r="B21">
+        <v>0.473132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1.3054100000000001E-2</v>
+      </c>
+      <c r="B22">
+        <v>0.47441499999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3.5786100000000001E-2</v>
+      </c>
+      <c r="B23">
+        <v>0.47379700000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5.8513200000000001E-2</v>
+      </c>
+      <c r="B24">
+        <v>0.47381400000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9.0336E-2</v>
+      </c>
+      <c r="B25">
+        <v>0.47320200000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.11457299999999999</v>
+      </c>
+      <c r="B26">
+        <v>0.47385699999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.13883000000000001</v>
+      </c>
+      <c r="B27">
+        <v>0.47196700000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.15851699999999999</v>
+      </c>
+      <c r="B28">
+        <v>0.47325400000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.196377</v>
+      </c>
+      <c r="B29">
+        <v>0.475827</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.23880999999999999</v>
+      </c>
+      <c r="B30">
+        <v>0.47458699999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.29486099999999998</v>
+      </c>
+      <c r="B31">
+        <v>0.47590199999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.33125300000000002</v>
+      </c>
+      <c r="B32">
+        <v>0.47211399999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.36004599999999998</v>
+      </c>
+      <c r="B33">
+        <v>0.47149999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.39943000000000001</v>
+      </c>
+      <c r="B34">
+        <v>0.472802</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.45092500000000002</v>
+      </c>
+      <c r="B35">
+        <v>0.475385</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.484288</v>
+      </c>
+      <c r="B36">
+        <v>0.47159499999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0.535798</v>
+      </c>
+      <c r="B37">
+        <v>0.47227000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0.57216599999999995</v>
+      </c>
+      <c r="B38">
+        <v>0.47166200000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0.61156900000000003</v>
+      </c>
+      <c r="B39">
+        <v>0.47042</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.64184799999999997</v>
+      </c>
+      <c r="B40">
+        <v>0.47362300000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0.663045</v>
+      </c>
+      <c r="B41">
+        <v>0.475547</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0.68124200000000001</v>
+      </c>
+      <c r="B42">
+        <v>0.47365299999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0.71003899999999998</v>
+      </c>
+      <c r="B43">
+        <v>0.47240300000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0.73575299999999999</v>
+      </c>
+      <c r="B44">
+        <v>0.47814600000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0.77667600000000003</v>
+      </c>
+      <c r="B45">
+        <v>0.47627000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0.82367999999999997</v>
+      </c>
+      <c r="B46">
+        <v>0.471854</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>0.86611300000000002</v>
+      </c>
+      <c r="B47">
+        <v>0.47061500000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0.91003299999999998</v>
+      </c>
+      <c r="B48">
+        <v>0.473192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0.95849300000000004</v>
+      </c>
+      <c r="B49">
+        <v>0.47640900000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0.98275999999999997</v>
+      </c>
+      <c r="B50">
+        <v>0.47324699999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1.0206599999999999</v>
+      </c>
+      <c r="B51">
+        <v>0.47009699999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1.0479099999999999</v>
+      </c>
+      <c r="B52">
+        <v>0.47393299999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1.1054999999999999</v>
+      </c>
+      <c r="B53">
+        <v>0.47143299999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1.1676</v>
+      </c>
+      <c r="B54">
+        <v>0.474024</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1.2130799999999999</v>
+      </c>
+      <c r="B55">
+        <v>0.47151500000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1.25095</v>
+      </c>
+      <c r="B56">
+        <v>0.47281600000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1.30246</v>
+      </c>
+      <c r="B57">
+        <v>0.47285500000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1.3539600000000001</v>
+      </c>
+      <c r="B58">
+        <v>0.47543800000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1.4009400000000001</v>
+      </c>
+      <c r="B59">
+        <v>0.47293099999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1.4418800000000001</v>
+      </c>
+      <c r="B60">
+        <v>0.46978199999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1.47973</v>
+      </c>
+      <c r="B61">
+        <v>0.47362700000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1.5191600000000001</v>
+      </c>
+      <c r="B62">
+        <v>0.46856900000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1.56159</v>
+      </c>
+      <c r="B63">
+        <v>0.46733000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1.6070199999999999</v>
+      </c>
+      <c r="B64">
+        <v>0.47117999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1.64944</v>
+      </c>
+      <c r="B65">
+        <v>0.47184799999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1.7070099999999999</v>
+      </c>
+      <c r="B66">
+        <v>0.47189199999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1.7645999999999999</v>
+      </c>
+      <c r="B67">
+        <v>0.470028</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1.8040099999999999</v>
+      </c>
+      <c r="B68">
+        <v>0.46878700000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1.8403799999999999</v>
+      </c>
+      <c r="B69">
+        <v>0.46690700000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1.88432</v>
+      </c>
+      <c r="B70">
+        <v>0.46694000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1.9494499999999999</v>
+      </c>
+      <c r="B71">
+        <v>0.46953400000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2.0161199999999999</v>
+      </c>
+      <c r="B72">
+        <v>0.47022000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2.0555300000000001</v>
+      </c>
+      <c r="B73">
+        <v>0.46770699999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2.1313</v>
+      </c>
+      <c r="B74">
+        <v>0.46585700000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2.1797900000000001</v>
+      </c>
+      <c r="B75">
+        <v>0.465258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2.2161400000000002</v>
+      </c>
+      <c r="B76">
+        <v>0.46719300000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2.2601200000000001</v>
+      </c>
+      <c r="B77">
+        <v>0.46150400000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2.2995399999999999</v>
+      </c>
+      <c r="B78">
+        <v>0.45899000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2.3298899999999998</v>
+      </c>
+      <c r="B79">
+        <v>0.45201799999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2.35114</v>
+      </c>
+      <c r="B80">
+        <v>0.44758199999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2.3708900000000002</v>
+      </c>
+      <c r="B81">
+        <v>0.43996600000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2.4012899999999999</v>
+      </c>
+      <c r="B82">
+        <v>0.42727100000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2.4150100000000001</v>
+      </c>
+      <c r="B83">
+        <v>0.41710599999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2.4272300000000002</v>
+      </c>
+      <c r="B84">
+        <v>0.40312500000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2.4470100000000001</v>
+      </c>
+      <c r="B85">
+        <v>0.39233000000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2.4577300000000002</v>
+      </c>
+      <c r="B86">
+        <v>0.37771100000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2.4683999999999999</v>
+      </c>
+      <c r="B87">
+        <v>0.369452</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2.48522</v>
+      </c>
+      <c r="B88">
+        <v>0.34911500000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>2.4929700000000001</v>
+      </c>
+      <c r="B89">
+        <v>0.32622800000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2.5113099999999999</v>
+      </c>
+      <c r="B90">
+        <v>0.305892</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>2.5205799999999998</v>
+      </c>
+      <c r="B91">
+        <v>0.28236899999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>2.5282800000000001</v>
+      </c>
+      <c r="B92">
+        <v>0.26520500000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2.5390199999999998</v>
+      </c>
+      <c r="B93">
+        <v>0.24867900000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>2.5528400000000002</v>
+      </c>
+      <c r="B94">
+        <v>0.224524</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2.56054</v>
+      </c>
+      <c r="B95">
+        <v>0.20735999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>2.5668299999999999</v>
+      </c>
+      <c r="B96">
+        <v>0.17811199999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>2.5730400000000002</v>
+      </c>
+      <c r="B97">
+        <v>0.15776699999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2.5807600000000002</v>
+      </c>
+      <c r="B98">
+        <v>0.13933100000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2.5900099999999999</v>
+      </c>
+      <c r="B99">
+        <v>0.118352</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2.5977800000000002</v>
+      </c>
+      <c r="B100">
+        <v>9.2284699999999997E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>2.60554</v>
+      </c>
+      <c r="B101">
+        <v>6.81253E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2.61178</v>
+      </c>
+      <c r="B102">
+        <v>4.5236499999999999E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>2.6194999999999999</v>
+      </c>
+      <c r="B103">
+        <v>2.6164400000000001E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>2.6212</v>
+      </c>
+      <c r="B104">
+        <v>1.36436E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>